<commit_message>
arreglando el excel del formato
</commit_message>
<xml_diff>
--- a/DLMallas/Content/Formato.xlsx
+++ b/DLMallas/Content/Formato.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Juanito\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Jaigle\maia\DLMallas\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD679EA8-438A-4CFA-9DA6-2C3369411FBB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9244A111-FBA0-4DF0-8446-7A8FCEE800A6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{A6BDA684-CA99-4418-91A4-DAC6D7765073}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Ruf</t>
+    <t>Rut</t>
   </si>
 </sst>
 </file>
@@ -388,9 +388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E83992-DF12-4B20-8B49-CEAAA6DA4C62}">
   <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>